<commit_message>
Update 4. Oblastný turnaj mládeže Zvolen 7.4.2019.xlsx
</commit_message>
<xml_diff>
--- a/stahovanie/4. Oblastný turnaj mládeže Zvolen 7.4.2019.xlsx
+++ b/stahovanie/4. Oblastný turnaj mládeže Zvolen 7.4.2019.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\obstz-zvolen.github.io\stahovanie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB5E9CC3-F18F-4193-9EFB-BB5782776612}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA9B689E-F989-457C-B293-E58AFFEA0CC4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prezenčná listina" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="115">
   <si>
     <t>Por.č.</t>
   </si>
@@ -360,6 +360,15 @@
   </si>
   <si>
     <t>2:15</t>
+  </si>
+  <si>
+    <t>Matúš Konôpka</t>
+  </si>
+  <si>
+    <t>Matúš Nagy</t>
+  </si>
+  <si>
+    <t>Hontianske Nemce</t>
   </si>
 </sst>
 </file>
@@ -1527,7 +1536,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="179">
+  <cellXfs count="185">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1680,19 +1689,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="72" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="9" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="14" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
@@ -1718,6 +1718,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="9" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1727,34 +1730,53 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="14" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="13" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="14" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="14" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="13" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="14" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="14" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1762,93 +1784,80 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="11" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="75" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="66" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="67" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="15" fillId="0" borderId="74" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="74" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="20" fontId="15" fillId="0" borderId="74" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="19" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="75" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="62" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="justify"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="justify"/>
     </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="66" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="67" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="19" fillId="0" borderId="74" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="68" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="69" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="78" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="71" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="justify"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="76" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="68" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="69" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="9" fillId="3" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1876,36 +1885,23 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="20" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1918,7 +1914,15 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1933,6 +1937,7 @@
     <xf numFmtId="49" fontId="9" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1940,20 +1945,34 @@
     <xf numFmtId="49" fontId="19" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="65" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="78" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="76" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2272,8 +2291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -2471,12 +2490,14 @@
         <v>19</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>73</v>
+        <v>113</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="43"/>
+      <c r="D16" s="43">
+        <v>2009</v>
+      </c>
       <c r="E16" s="3"/>
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1">
@@ -2561,7 +2582,9 @@
       <c r="B22" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C22" s="1"/>
+      <c r="C22" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="D22" s="43">
         <v>2009</v>
       </c>
@@ -2616,9 +2639,15 @@
       <c r="A26" s="42">
         <v>22</v>
       </c>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="43"/>
+      <c r="B26" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D26" s="43">
+        <v>2009</v>
+      </c>
       <c r="E26" s="3"/>
     </row>
     <row r="27" spans="1:5" thickBot="1">
@@ -2650,7 +2679,7 @@
   <dimension ref="A1:J52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10:J11"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -2660,7 +2689,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" customHeight="1"/>
     <row r="2" spans="1:10" ht="21" customHeight="1">
-      <c r="A2" s="66"/>
+      <c r="A2" s="62"/>
       <c r="B2" s="63"/>
       <c r="C2" s="63"/>
       <c r="D2" s="63"/>
@@ -2678,7 +2707,7 @@
       <c r="D3" s="8"/>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
-      <c r="G3" s="67"/>
+      <c r="G3" s="64"/>
       <c r="H3" s="63"/>
       <c r="I3" s="63"/>
       <c r="J3" s="63"/>
@@ -2696,10 +2725,10 @@
       <c r="J4" s="11"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A5" s="81" t="s">
+      <c r="A5" s="79" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="82"/>
+      <c r="B5" s="80"/>
       <c r="C5" s="12" t="s">
         <v>30</v>
       </c>
@@ -2726,172 +2755,180 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A6" s="78">
+      <c r="A6" s="76">
         <v>1</v>
       </c>
-      <c r="B6" s="74" t="s">
+      <c r="B6" s="71" t="s">
         <v>80</v>
       </c>
-      <c r="C6" s="75"/>
-      <c r="D6" s="110" t="s">
+      <c r="C6" s="72"/>
+      <c r="D6" s="109" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="87" t="s">
+      <c r="E6" s="101" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="87" t="s">
+      <c r="F6" s="101" t="s">
         <v>35</v>
       </c>
-      <c r="G6" s="98" t="s">
+      <c r="G6" s="103" t="s">
         <v>36</v>
       </c>
-      <c r="H6" s="89" t="s">
+      <c r="H6" s="98" t="s">
         <v>37</v>
       </c>
-      <c r="I6" s="102" t="s">
+      <c r="I6" s="93" t="s">
         <v>42</v>
       </c>
-      <c r="J6" s="93" t="s">
+      <c r="J6" s="89" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A7" s="79"/>
-      <c r="B7" s="104"/>
-      <c r="C7" s="70"/>
-      <c r="D7" s="79"/>
-      <c r="E7" s="88"/>
-      <c r="F7" s="88"/>
-      <c r="G7" s="99"/>
-      <c r="H7" s="90"/>
-      <c r="I7" s="88"/>
-      <c r="J7" s="94"/>
+      <c r="A7" s="77"/>
+      <c r="B7" s="113" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="67"/>
+      <c r="D7" s="77"/>
+      <c r="E7" s="94"/>
+      <c r="F7" s="94"/>
+      <c r="G7" s="104"/>
+      <c r="H7" s="99"/>
+      <c r="I7" s="94"/>
+      <c r="J7" s="90"/>
     </row>
     <row r="8" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A8" s="76">
+      <c r="A8" s="73">
         <v>2</v>
       </c>
-      <c r="B8" s="106" t="s">
+      <c r="B8" s="107" t="s">
         <v>83</v>
       </c>
       <c r="C8" s="63"/>
-      <c r="D8" s="109" t="s">
+      <c r="D8" s="108" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="85" t="s">
+      <c r="E8" s="100" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="87" t="s">
+      <c r="F8" s="101" t="s">
         <v>39</v>
       </c>
-      <c r="G8" s="98" t="s">
+      <c r="G8" s="103" t="s">
         <v>39</v>
       </c>
-      <c r="H8" s="100" t="s">
+      <c r="H8" s="96" t="s">
         <v>88</v>
       </c>
-      <c r="I8" s="83" t="s">
+      <c r="I8" s="82" t="s">
         <v>43</v>
       </c>
-      <c r="J8" s="95" t="s">
+      <c r="J8" s="91" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A9" s="80"/>
-      <c r="B9" s="69"/>
-      <c r="C9" s="70"/>
-      <c r="D9" s="80"/>
-      <c r="E9" s="86"/>
-      <c r="F9" s="88"/>
-      <c r="G9" s="99"/>
-      <c r="H9" s="103"/>
-      <c r="I9" s="86"/>
-      <c r="J9" s="96"/>
+      <c r="A9" s="78"/>
+      <c r="B9" s="66" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="67"/>
+      <c r="D9" s="78"/>
+      <c r="E9" s="95"/>
+      <c r="F9" s="94"/>
+      <c r="G9" s="104"/>
+      <c r="H9" s="97"/>
+      <c r="I9" s="95"/>
+      <c r="J9" s="92"/>
     </row>
     <row r="10" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A10" s="78">
+      <c r="A10" s="76">
         <v>3</v>
       </c>
-      <c r="B10" s="74" t="s">
+      <c r="B10" s="71" t="s">
         <v>84</v>
       </c>
-      <c r="C10" s="75"/>
-      <c r="D10" s="111" t="s">
+      <c r="C10" s="72"/>
+      <c r="D10" s="110" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="89" t="s">
+      <c r="E10" s="98" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="105" t="s">
+      <c r="F10" s="106" t="s">
         <v>34</v>
       </c>
-      <c r="G10" s="98" t="s">
+      <c r="G10" s="103" t="s">
         <v>36</v>
       </c>
-      <c r="H10" s="89" t="s">
+      <c r="H10" s="98" t="s">
         <v>87</v>
       </c>
-      <c r="I10" s="102" t="s">
+      <c r="I10" s="93" t="s">
         <v>57</v>
       </c>
-      <c r="J10" s="93" t="s">
+      <c r="J10" s="89" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A11" s="79"/>
-      <c r="B11" s="73"/>
+      <c r="A11" s="77"/>
+      <c r="B11" s="70" t="s">
+        <v>114</v>
+      </c>
       <c r="C11" s="63"/>
-      <c r="D11" s="79"/>
-      <c r="E11" s="90"/>
-      <c r="F11" s="88"/>
-      <c r="G11" s="99"/>
-      <c r="H11" s="90"/>
-      <c r="I11" s="88"/>
-      <c r="J11" s="94"/>
+      <c r="D11" s="77"/>
+      <c r="E11" s="99"/>
+      <c r="F11" s="94"/>
+      <c r="G11" s="104"/>
+      <c r="H11" s="99"/>
+      <c r="I11" s="94"/>
+      <c r="J11" s="90"/>
     </row>
     <row r="12" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A12" s="76">
+      <c r="A12" s="73">
         <v>4</v>
       </c>
-      <c r="B12" s="71" t="s">
+      <c r="B12" s="68" t="s">
         <v>85</v>
       </c>
-      <c r="C12" s="72"/>
-      <c r="D12" s="100" t="s">
+      <c r="C12" s="69"/>
+      <c r="D12" s="96" t="s">
         <v>41</v>
       </c>
-      <c r="E12" s="83" t="s">
+      <c r="E12" s="82" t="s">
         <v>35</v>
       </c>
-      <c r="F12" s="100" t="s">
+      <c r="F12" s="96" t="s">
         <v>41</v>
       </c>
-      <c r="G12" s="97" t="s">
+      <c r="G12" s="102" t="s">
         <v>34</v>
       </c>
-      <c r="H12" s="100" t="s">
+      <c r="H12" s="96" t="s">
         <v>86</v>
       </c>
-      <c r="I12" s="83" t="s">
+      <c r="I12" s="82" t="s">
         <v>58</v>
       </c>
-      <c r="J12" s="91" t="s">
+      <c r="J12" s="87" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A13" s="77"/>
-      <c r="B13" s="112"/>
-      <c r="C13" s="113"/>
-      <c r="D13" s="101"/>
-      <c r="E13" s="84"/>
-      <c r="F13" s="101"/>
-      <c r="G13" s="92"/>
-      <c r="H13" s="101"/>
-      <c r="I13" s="84"/>
-      <c r="J13" s="92"/>
+      <c r="A13" s="74"/>
+      <c r="B13" s="111" t="s">
+        <v>114</v>
+      </c>
+      <c r="C13" s="112"/>
+      <c r="D13" s="105"/>
+      <c r="E13" s="83"/>
+      <c r="F13" s="105"/>
+      <c r="G13" s="88"/>
+      <c r="H13" s="105"/>
+      <c r="I13" s="83"/>
+      <c r="J13" s="88"/>
     </row>
     <row r="14" spans="1:10" ht="15.75" customHeight="1">
       <c r="A14" s="22"/>
@@ -2930,7 +2967,7 @@
       <c r="J15" s="29"/>
     </row>
     <row r="16" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A16" s="62"/>
+      <c r="A16" s="75"/>
       <c r="B16" s="63"/>
       <c r="C16" s="31"/>
       <c r="D16" s="32"/>
@@ -2942,20 +2979,20 @@
       <c r="J16" s="32"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A17" s="68"/>
-      <c r="B17" s="107"/>
+      <c r="A17" s="65"/>
+      <c r="B17" s="85"/>
       <c r="C17" s="63"/>
-      <c r="D17" s="62"/>
-      <c r="E17" s="65"/>
-      <c r="F17" s="65"/>
-      <c r="G17" s="65"/>
-      <c r="H17" s="64"/>
-      <c r="I17" s="64"/>
-      <c r="J17" s="64"/>
+      <c r="D17" s="75"/>
+      <c r="E17" s="84"/>
+      <c r="F17" s="84"/>
+      <c r="G17" s="84"/>
+      <c r="H17" s="81"/>
+      <c r="I17" s="81"/>
+      <c r="J17" s="81"/>
     </row>
     <row r="18" spans="1:10" ht="15.75" customHeight="1">
       <c r="A18" s="63"/>
-      <c r="B18" s="108"/>
+      <c r="B18" s="86"/>
       <c r="C18" s="63"/>
       <c r="D18" s="63"/>
       <c r="E18" s="63"/>
@@ -2966,20 +3003,20 @@
       <c r="J18" s="63"/>
     </row>
     <row r="19" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A19" s="68"/>
-      <c r="B19" s="107"/>
+      <c r="A19" s="65"/>
+      <c r="B19" s="85"/>
       <c r="C19" s="63"/>
-      <c r="D19" s="64"/>
-      <c r="E19" s="62"/>
-      <c r="F19" s="65"/>
-      <c r="G19" s="65"/>
-      <c r="H19" s="64"/>
-      <c r="I19" s="64"/>
-      <c r="J19" s="64"/>
+      <c r="D19" s="81"/>
+      <c r="E19" s="75"/>
+      <c r="F19" s="84"/>
+      <c r="G19" s="84"/>
+      <c r="H19" s="81"/>
+      <c r="I19" s="81"/>
+      <c r="J19" s="81"/>
     </row>
     <row r="20" spans="1:10" ht="15.75" customHeight="1">
       <c r="A20" s="63"/>
-      <c r="B20" s="108"/>
+      <c r="B20" s="86"/>
       <c r="C20" s="63"/>
       <c r="D20" s="63"/>
       <c r="E20" s="63"/>
@@ -2990,20 +3027,20 @@
       <c r="J20" s="63"/>
     </row>
     <row r="21" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A21" s="68"/>
-      <c r="B21" s="107"/>
+      <c r="A21" s="65"/>
+      <c r="B21" s="85"/>
       <c r="C21" s="63"/>
-      <c r="D21" s="64"/>
-      <c r="E21" s="64"/>
-      <c r="F21" s="62"/>
-      <c r="G21" s="65"/>
-      <c r="H21" s="64"/>
-      <c r="I21" s="64"/>
-      <c r="J21" s="64"/>
+      <c r="D21" s="81"/>
+      <c r="E21" s="81"/>
+      <c r="F21" s="75"/>
+      <c r="G21" s="84"/>
+      <c r="H21" s="81"/>
+      <c r="I21" s="81"/>
+      <c r="J21" s="81"/>
     </row>
     <row r="22" spans="1:10" ht="15.75" customHeight="1">
       <c r="A22" s="63"/>
-      <c r="B22" s="108"/>
+      <c r="B22" s="86"/>
       <c r="C22" s="63"/>
       <c r="D22" s="63"/>
       <c r="E22" s="63"/>
@@ -3014,20 +3051,20 @@
       <c r="J22" s="63"/>
     </row>
     <row r="23" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A23" s="68"/>
-      <c r="B23" s="107"/>
+      <c r="A23" s="65"/>
+      <c r="B23" s="85"/>
       <c r="C23" s="63"/>
-      <c r="D23" s="64"/>
-      <c r="E23" s="64"/>
-      <c r="F23" s="64"/>
-      <c r="G23" s="62"/>
-      <c r="H23" s="64"/>
-      <c r="I23" s="64"/>
-      <c r="J23" s="64"/>
+      <c r="D23" s="81"/>
+      <c r="E23" s="81"/>
+      <c r="F23" s="81"/>
+      <c r="G23" s="75"/>
+      <c r="H23" s="81"/>
+      <c r="I23" s="81"/>
+      <c r="J23" s="81"/>
     </row>
     <row r="24" spans="1:10" ht="15.75" customHeight="1">
       <c r="A24" s="63"/>
-      <c r="B24" s="108"/>
+      <c r="B24" s="86"/>
       <c r="C24" s="63"/>
       <c r="D24" s="63"/>
       <c r="E24" s="63"/>
@@ -3062,7 +3099,7 @@
       <c r="J26" s="29"/>
     </row>
     <row r="27" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A27" s="62"/>
+      <c r="A27" s="75"/>
       <c r="B27" s="63"/>
       <c r="C27" s="31"/>
       <c r="D27" s="32"/>
@@ -3074,20 +3111,20 @@
       <c r="J27" s="32"/>
     </row>
     <row r="28" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A28" s="68"/>
-      <c r="B28" s="107"/>
+      <c r="A28" s="65"/>
+      <c r="B28" s="85"/>
       <c r="C28" s="63"/>
-      <c r="D28" s="62"/>
+      <c r="D28" s="75"/>
       <c r="E28" s="34"/>
       <c r="F28" s="34"/>
       <c r="G28" s="34"/>
-      <c r="H28" s="64"/>
-      <c r="I28" s="64"/>
-      <c r="J28" s="64"/>
+      <c r="H28" s="81"/>
+      <c r="I28" s="81"/>
+      <c r="J28" s="81"/>
     </row>
     <row r="29" spans="1:10" ht="15.75" customHeight="1">
       <c r="A29" s="63"/>
-      <c r="B29" s="108"/>
+      <c r="B29" s="86"/>
       <c r="C29" s="63"/>
       <c r="D29" s="63"/>
       <c r="E29" s="37"/>
@@ -3098,20 +3135,20 @@
       <c r="J29" s="63"/>
     </row>
     <row r="30" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A30" s="68"/>
-      <c r="B30" s="107"/>
+      <c r="A30" s="65"/>
+      <c r="B30" s="85"/>
       <c r="C30" s="63"/>
-      <c r="D30" s="64"/>
-      <c r="E30" s="62"/>
+      <c r="D30" s="81"/>
+      <c r="E30" s="75"/>
       <c r="F30" s="34"/>
       <c r="G30" s="34"/>
-      <c r="H30" s="64"/>
-      <c r="I30" s="64"/>
-      <c r="J30" s="64"/>
+      <c r="H30" s="81"/>
+      <c r="I30" s="81"/>
+      <c r="J30" s="81"/>
     </row>
     <row r="31" spans="1:10" ht="15.75" customHeight="1">
       <c r="A31" s="63"/>
-      <c r="B31" s="108"/>
+      <c r="B31" s="86"/>
       <c r="C31" s="63"/>
       <c r="D31" s="63"/>
       <c r="E31" s="63"/>
@@ -3122,20 +3159,20 @@
       <c r="J31" s="63"/>
     </row>
     <row r="32" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A32" s="68"/>
-      <c r="B32" s="107"/>
+      <c r="A32" s="65"/>
+      <c r="B32" s="85"/>
       <c r="C32" s="63"/>
-      <c r="D32" s="64"/>
-      <c r="E32" s="64"/>
-      <c r="F32" s="62"/>
+      <c r="D32" s="81"/>
+      <c r="E32" s="81"/>
+      <c r="F32" s="75"/>
       <c r="G32" s="34"/>
-      <c r="H32" s="64"/>
-      <c r="I32" s="64"/>
-      <c r="J32" s="64"/>
+      <c r="H32" s="81"/>
+      <c r="I32" s="81"/>
+      <c r="J32" s="81"/>
     </row>
     <row r="33" spans="1:10" ht="15.75" customHeight="1">
       <c r="A33" s="63"/>
-      <c r="B33" s="108"/>
+      <c r="B33" s="86"/>
       <c r="C33" s="63"/>
       <c r="D33" s="63"/>
       <c r="E33" s="63"/>
@@ -3146,20 +3183,20 @@
       <c r="J33" s="63"/>
     </row>
     <row r="34" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A34" s="68"/>
-      <c r="B34" s="107"/>
+      <c r="A34" s="65"/>
+      <c r="B34" s="85"/>
       <c r="C34" s="63"/>
-      <c r="D34" s="64"/>
-      <c r="E34" s="64"/>
-      <c r="F34" s="64"/>
-      <c r="G34" s="62"/>
-      <c r="H34" s="64"/>
-      <c r="I34" s="64"/>
-      <c r="J34" s="64"/>
+      <c r="D34" s="81"/>
+      <c r="E34" s="81"/>
+      <c r="F34" s="81"/>
+      <c r="G34" s="75"/>
+      <c r="H34" s="81"/>
+      <c r="I34" s="81"/>
+      <c r="J34" s="81"/>
     </row>
     <row r="35" spans="1:10" ht="15.75" customHeight="1">
       <c r="A35" s="63"/>
-      <c r="B35" s="108"/>
+      <c r="B35" s="86"/>
       <c r="C35" s="63"/>
       <c r="D35" s="63"/>
       <c r="E35" s="63"/>
@@ -3194,7 +3231,7 @@
       <c r="J37" s="29"/>
     </row>
     <row r="38" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A38" s="62"/>
+      <c r="A38" s="75"/>
       <c r="B38" s="63"/>
       <c r="C38" s="31"/>
       <c r="D38" s="32"/>
@@ -3206,20 +3243,20 @@
       <c r="J38" s="32"/>
     </row>
     <row r="39" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A39" s="68"/>
-      <c r="B39" s="107"/>
+      <c r="A39" s="65"/>
+      <c r="B39" s="85"/>
       <c r="C39" s="63"/>
-      <c r="D39" s="62"/>
+      <c r="D39" s="75"/>
       <c r="E39" s="34"/>
       <c r="F39" s="34"/>
       <c r="G39" s="34"/>
-      <c r="H39" s="64"/>
-      <c r="I39" s="64"/>
-      <c r="J39" s="64"/>
+      <c r="H39" s="81"/>
+      <c r="I39" s="81"/>
+      <c r="J39" s="81"/>
     </row>
     <row r="40" spans="1:10" ht="15.75" customHeight="1">
       <c r="A40" s="63"/>
-      <c r="B40" s="108"/>
+      <c r="B40" s="86"/>
       <c r="C40" s="63"/>
       <c r="D40" s="63"/>
       <c r="E40" s="37"/>
@@ -3230,20 +3267,20 @@
       <c r="J40" s="63"/>
     </row>
     <row r="41" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A41" s="68"/>
-      <c r="B41" s="107"/>
+      <c r="A41" s="65"/>
+      <c r="B41" s="85"/>
       <c r="C41" s="63"/>
-      <c r="D41" s="64"/>
-      <c r="E41" s="62"/>
+      <c r="D41" s="81"/>
+      <c r="E41" s="75"/>
       <c r="F41" s="34"/>
       <c r="G41" s="34"/>
-      <c r="H41" s="64"/>
-      <c r="I41" s="64"/>
-      <c r="J41" s="64"/>
+      <c r="H41" s="81"/>
+      <c r="I41" s="81"/>
+      <c r="J41" s="81"/>
     </row>
     <row r="42" spans="1:10" ht="15.75" customHeight="1">
       <c r="A42" s="63"/>
-      <c r="B42" s="108"/>
+      <c r="B42" s="86"/>
       <c r="C42" s="63"/>
       <c r="D42" s="63"/>
       <c r="E42" s="63"/>
@@ -3254,20 +3291,20 @@
       <c r="J42" s="63"/>
     </row>
     <row r="43" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A43" s="68"/>
-      <c r="B43" s="107"/>
+      <c r="A43" s="65"/>
+      <c r="B43" s="85"/>
       <c r="C43" s="63"/>
-      <c r="D43" s="64"/>
-      <c r="E43" s="64"/>
-      <c r="F43" s="62"/>
+      <c r="D43" s="81"/>
+      <c r="E43" s="81"/>
+      <c r="F43" s="75"/>
       <c r="G43" s="34"/>
-      <c r="H43" s="64"/>
-      <c r="I43" s="64"/>
-      <c r="J43" s="64"/>
+      <c r="H43" s="81"/>
+      <c r="I43" s="81"/>
+      <c r="J43" s="81"/>
     </row>
     <row r="44" spans="1:10" ht="15.75" customHeight="1">
       <c r="A44" s="63"/>
-      <c r="B44" s="108"/>
+      <c r="B44" s="86"/>
       <c r="C44" s="63"/>
       <c r="D44" s="63"/>
       <c r="E44" s="63"/>
@@ -3278,20 +3315,20 @@
       <c r="J44" s="63"/>
     </row>
     <row r="45" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A45" s="68"/>
-      <c r="B45" s="107"/>
+      <c r="A45" s="65"/>
+      <c r="B45" s="85"/>
       <c r="C45" s="63"/>
-      <c r="D45" s="64"/>
-      <c r="E45" s="64"/>
-      <c r="F45" s="64"/>
-      <c r="G45" s="62"/>
-      <c r="H45" s="64"/>
-      <c r="I45" s="64"/>
-      <c r="J45" s="64"/>
+      <c r="D45" s="81"/>
+      <c r="E45" s="81"/>
+      <c r="F45" s="81"/>
+      <c r="G45" s="75"/>
+      <c r="H45" s="81"/>
+      <c r="I45" s="81"/>
+      <c r="J45" s="81"/>
     </row>
     <row r="46" spans="1:10" ht="15.75" customHeight="1">
       <c r="A46" s="63"/>
-      <c r="B46" s="108"/>
+      <c r="B46" s="86"/>
       <c r="C46" s="63"/>
       <c r="D46" s="63"/>
       <c r="E46" s="63"/>
@@ -3394,6 +3431,10 @@
     <mergeCell ref="F32:F33"/>
     <mergeCell ref="B40:C40"/>
     <mergeCell ref="B39:C39"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B30:C30"/>
     <mergeCell ref="F45:F46"/>
     <mergeCell ref="G45:G46"/>
     <mergeCell ref="I41:I42"/>
@@ -3413,12 +3454,9 @@
     <mergeCell ref="D45:D46"/>
     <mergeCell ref="B44:C44"/>
     <mergeCell ref="D43:D44"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="E41:E42"/>
     <mergeCell ref="D23:D24"/>
     <mergeCell ref="D21:D22"/>
     <mergeCell ref="D17:D18"/>
@@ -3431,23 +3469,44 @@
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="F10:F11"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="G8:G9"/>
     <mergeCell ref="G10:G11"/>
     <mergeCell ref="H10:H11"/>
     <mergeCell ref="H12:H13"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="I23:I24"/>
+    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="I19:I20"/>
     <mergeCell ref="G21:G22"/>
     <mergeCell ref="G19:G20"/>
     <mergeCell ref="G23:G24"/>
@@ -3456,30 +3515,8 @@
     <mergeCell ref="I8:I9"/>
     <mergeCell ref="H8:H9"/>
     <mergeCell ref="H6:H7"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="E45:E46"/>
-    <mergeCell ref="E43:E44"/>
-    <mergeCell ref="E41:E42"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="J23:J24"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="J21:J22"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="I23:I24"/>
-    <mergeCell ref="I21:I22"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="H21:H22"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="I10:I11"/>
     <mergeCell ref="A45:A46"/>
     <mergeCell ref="A43:A44"/>
     <mergeCell ref="A34:A35"/>
@@ -3494,10 +3531,6 @@
     <mergeCell ref="B46:C46"/>
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="B33:C33"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="F17:F18"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="G3:J3"/>
     <mergeCell ref="A19:A20"/>
@@ -3518,6 +3551,10 @@
     <mergeCell ref="E21:E22"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="E17:E18"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="J23:J24"/>
+    <mergeCell ref="J19:J20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3527,8 +3564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9060612D-BEF6-4965-B8AC-CD7B357C81D3}">
   <dimension ref="B1:O22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17:J18"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -3577,574 +3614,574 @@
       </c>
     </row>
     <row r="3" spans="2:15" ht="21.75" customHeight="1">
-      <c r="B3" s="116" t="s">
+      <c r="B3" s="123" t="s">
         <v>92</v>
       </c>
-      <c r="C3" s="125"/>
-      <c r="D3" s="118" t="s">
+      <c r="C3" s="120"/>
+      <c r="D3" s="122" t="s">
         <v>36</v>
       </c>
-      <c r="E3" s="118" t="s">
+      <c r="E3" s="122" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="118" t="s">
+      <c r="F3" s="122" t="s">
         <v>55</v>
       </c>
-      <c r="G3" s="118" t="s">
+      <c r="G3" s="122" t="s">
         <v>36</v>
       </c>
-      <c r="H3" s="118" t="s">
+      <c r="H3" s="122" t="s">
         <v>35</v>
       </c>
-      <c r="I3" s="118" t="s">
+      <c r="I3" s="122" t="s">
         <v>36</v>
       </c>
-      <c r="J3" s="118" t="s">
+      <c r="J3" s="122" t="s">
         <v>36</v>
       </c>
-      <c r="K3" s="118" t="s">
+      <c r="K3" s="122" t="s">
         <v>35</v>
       </c>
-      <c r="L3" s="119" t="s">
+      <c r="L3" s="125" t="s">
         <v>36</v>
       </c>
-      <c r="M3" s="121"/>
-      <c r="N3" s="114" t="s">
+      <c r="M3" s="115"/>
+      <c r="N3" s="118" t="s">
         <v>59</v>
       </c>
-      <c r="O3" s="114" t="s">
+      <c r="O3" s="118" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="4" spans="2:15" ht="21.75" customHeight="1" thickBot="1">
-      <c r="B4" s="117"/>
-      <c r="C4" s="126"/>
-      <c r="D4" s="101"/>
-      <c r="E4" s="101"/>
-      <c r="F4" s="101"/>
-      <c r="G4" s="101"/>
-      <c r="H4" s="101"/>
-      <c r="I4" s="101"/>
-      <c r="J4" s="101"/>
-      <c r="K4" s="101"/>
-      <c r="L4" s="120"/>
-      <c r="M4" s="121"/>
-      <c r="N4" s="115"/>
-      <c r="O4" s="115"/>
+      <c r="B4" s="124"/>
+      <c r="C4" s="121"/>
+      <c r="D4" s="105"/>
+      <c r="E4" s="105"/>
+      <c r="F4" s="105"/>
+      <c r="G4" s="105"/>
+      <c r="H4" s="105"/>
+      <c r="I4" s="105"/>
+      <c r="J4" s="105"/>
+      <c r="K4" s="105"/>
+      <c r="L4" s="126"/>
+      <c r="M4" s="115"/>
+      <c r="N4" s="119"/>
+      <c r="O4" s="119"/>
     </row>
     <row r="5" spans="2:15" ht="21.75" customHeight="1">
-      <c r="B5" s="116" t="s">
+      <c r="B5" s="123" t="s">
         <v>93</v>
       </c>
-      <c r="C5" s="100" t="s">
+      <c r="C5" s="96" t="s">
         <v>41</v>
       </c>
-      <c r="D5" s="125"/>
-      <c r="E5" s="118" t="s">
+      <c r="D5" s="120"/>
+      <c r="E5" s="122" t="s">
         <v>41</v>
       </c>
-      <c r="F5" s="118" t="s">
+      <c r="F5" s="122" t="s">
         <v>41</v>
       </c>
-      <c r="G5" s="118" t="s">
+      <c r="G5" s="122" t="s">
         <v>36</v>
       </c>
-      <c r="H5" s="118" t="s">
+      <c r="H5" s="122" t="s">
         <v>35</v>
       </c>
-      <c r="I5" s="118" t="s">
+      <c r="I5" s="122" t="s">
         <v>36</v>
       </c>
-      <c r="J5" s="118" t="s">
+      <c r="J5" s="122" t="s">
         <v>36</v>
       </c>
-      <c r="K5" s="118" t="s">
+      <c r="K5" s="122" t="s">
         <v>41</v>
       </c>
-      <c r="L5" s="119" t="s">
+      <c r="L5" s="125" t="s">
         <v>36</v>
       </c>
-      <c r="M5" s="122">
+      <c r="M5" s="114">
         <v>0.63402777777777775</v>
       </c>
-      <c r="N5" s="123" t="s">
+      <c r="N5" s="116" t="s">
         <v>45</v>
       </c>
-      <c r="O5" s="114" t="s">
-        <v>60</v>
+      <c r="O5" s="118" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="2:15" ht="23.25" customHeight="1" thickBot="1">
-      <c r="B6" s="117"/>
-      <c r="C6" s="101"/>
-      <c r="D6" s="126"/>
-      <c r="E6" s="101"/>
-      <c r="F6" s="101"/>
-      <c r="G6" s="101"/>
-      <c r="H6" s="101"/>
-      <c r="I6" s="101"/>
-      <c r="J6" s="101"/>
-      <c r="K6" s="101"/>
-      <c r="L6" s="120"/>
-      <c r="M6" s="121"/>
-      <c r="N6" s="124"/>
-      <c r="O6" s="115"/>
+      <c r="B6" s="124"/>
+      <c r="C6" s="105"/>
+      <c r="D6" s="121"/>
+      <c r="E6" s="105"/>
+      <c r="F6" s="105"/>
+      <c r="G6" s="105"/>
+      <c r="H6" s="105"/>
+      <c r="I6" s="105"/>
+      <c r="J6" s="105"/>
+      <c r="K6" s="105"/>
+      <c r="L6" s="126"/>
+      <c r="M6" s="115"/>
+      <c r="N6" s="117"/>
+      <c r="O6" s="119"/>
     </row>
     <row r="7" spans="2:15" ht="23.25" customHeight="1">
-      <c r="B7" s="116" t="s">
+      <c r="B7" s="123" t="s">
         <v>94</v>
       </c>
-      <c r="C7" s="118" t="s">
+      <c r="C7" s="122" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="118" t="s">
+      <c r="D7" s="122" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="125"/>
-      <c r="F7" s="118" t="s">
+      <c r="E7" s="120"/>
+      <c r="F7" s="122" t="s">
         <v>55</v>
       </c>
-      <c r="G7" s="118" t="s">
+      <c r="G7" s="122" t="s">
         <v>36</v>
       </c>
-      <c r="H7" s="118" t="s">
+      <c r="H7" s="122" t="s">
         <v>35</v>
       </c>
-      <c r="I7" s="118" t="s">
+      <c r="I7" s="122" t="s">
         <v>36</v>
       </c>
-      <c r="J7" s="118" t="s">
+      <c r="J7" s="122" t="s">
         <v>36</v>
       </c>
-      <c r="K7" s="118" t="s">
+      <c r="K7" s="122" t="s">
         <v>35</v>
       </c>
-      <c r="L7" s="119" t="s">
+      <c r="L7" s="125" t="s">
         <v>36</v>
       </c>
       <c r="M7" s="127" t="s">
         <v>101</v>
       </c>
-      <c r="N7" s="123" t="s">
+      <c r="N7" s="116" t="s">
         <v>99</v>
       </c>
-      <c r="O7" s="114" t="s">
+      <c r="O7" s="118" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="8" spans="2:15" ht="21.75" customHeight="1" thickBot="1">
-      <c r="B8" s="117"/>
-      <c r="C8" s="101"/>
-      <c r="D8" s="101"/>
-      <c r="E8" s="126"/>
-      <c r="F8" s="101"/>
-      <c r="G8" s="101"/>
-      <c r="H8" s="101"/>
-      <c r="I8" s="101"/>
-      <c r="J8" s="101"/>
-      <c r="K8" s="101"/>
-      <c r="L8" s="120"/>
+      <c r="B8" s="124"/>
+      <c r="C8" s="105"/>
+      <c r="D8" s="105"/>
+      <c r="E8" s="121"/>
+      <c r="F8" s="105"/>
+      <c r="G8" s="105"/>
+      <c r="H8" s="105"/>
+      <c r="I8" s="105"/>
+      <c r="J8" s="105"/>
+      <c r="K8" s="105"/>
+      <c r="L8" s="126"/>
       <c r="M8" s="128"/>
-      <c r="N8" s="124"/>
-      <c r="O8" s="115"/>
+      <c r="N8" s="117"/>
+      <c r="O8" s="119"/>
     </row>
     <row r="9" spans="2:15" ht="21.75" customHeight="1">
-      <c r="B9" s="116" t="s">
+      <c r="B9" s="123" t="s">
         <v>95</v>
       </c>
-      <c r="C9" s="118" t="s">
+      <c r="C9" s="122" t="s">
         <v>52</v>
       </c>
-      <c r="D9" s="118" t="s">
+      <c r="D9" s="122" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="118" t="s">
+      <c r="E9" s="122" t="s">
         <v>52</v>
       </c>
-      <c r="F9" s="125"/>
-      <c r="G9" s="118" t="s">
+      <c r="F9" s="120"/>
+      <c r="G9" s="122" t="s">
         <v>36</v>
       </c>
-      <c r="H9" s="118" t="s">
+      <c r="H9" s="122" t="s">
         <v>35</v>
       </c>
-      <c r="I9" s="118" t="s">
+      <c r="I9" s="122" t="s">
         <v>36</v>
       </c>
-      <c r="J9" s="118" t="s">
+      <c r="J9" s="122" t="s">
         <v>36</v>
       </c>
-      <c r="K9" s="118" t="s">
+      <c r="K9" s="122" t="s">
         <v>36</v>
       </c>
-      <c r="L9" s="119" t="s">
+      <c r="L9" s="125" t="s">
         <v>36</v>
       </c>
-      <c r="M9" s="121"/>
-      <c r="N9" s="123" t="s">
+      <c r="M9" s="115"/>
+      <c r="N9" s="116" t="s">
         <v>100</v>
       </c>
-      <c r="O9" s="114" t="s">
+      <c r="O9" s="118" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="10" spans="2:15" ht="23.25" customHeight="1" thickBot="1">
-      <c r="B10" s="117"/>
-      <c r="C10" s="101"/>
-      <c r="D10" s="101"/>
-      <c r="E10" s="101"/>
-      <c r="F10" s="126"/>
-      <c r="G10" s="101"/>
-      <c r="H10" s="101"/>
-      <c r="I10" s="101"/>
-      <c r="J10" s="101"/>
-      <c r="K10" s="101"/>
-      <c r="L10" s="120"/>
-      <c r="M10" s="121"/>
-      <c r="N10" s="124"/>
-      <c r="O10" s="115"/>
+      <c r="B10" s="124"/>
+      <c r="C10" s="105"/>
+      <c r="D10" s="105"/>
+      <c r="E10" s="105"/>
+      <c r="F10" s="121"/>
+      <c r="G10" s="105"/>
+      <c r="H10" s="105"/>
+      <c r="I10" s="105"/>
+      <c r="J10" s="105"/>
+      <c r="K10" s="105"/>
+      <c r="L10" s="126"/>
+      <c r="M10" s="115"/>
+      <c r="N10" s="117"/>
+      <c r="O10" s="119"/>
     </row>
     <row r="11" spans="2:15" ht="23.25" customHeight="1">
-      <c r="B11" s="116" t="s">
+      <c r="B11" s="123" t="s">
         <v>73</v>
       </c>
-      <c r="C11" s="100" t="s">
+      <c r="C11" s="96" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="100" t="s">
+      <c r="D11" s="96" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="100" t="s">
+      <c r="E11" s="96" t="s">
         <v>41</v>
       </c>
-      <c r="F11" s="100" t="s">
+      <c r="F11" s="96" t="s">
         <v>41</v>
       </c>
-      <c r="G11" s="125"/>
-      <c r="H11" s="118" t="s">
+      <c r="G11" s="120"/>
+      <c r="H11" s="122" t="s">
         <v>39</v>
       </c>
-      <c r="I11" s="100" t="s">
+      <c r="I11" s="96" t="s">
         <v>41</v>
       </c>
-      <c r="J11" s="118" t="s">
+      <c r="J11" s="122" t="s">
         <v>36</v>
       </c>
-      <c r="K11" s="100" t="s">
+      <c r="K11" s="96" t="s">
         <v>41</v>
       </c>
-      <c r="L11" s="119" t="s">
+      <c r="L11" s="125" t="s">
         <v>55</v>
       </c>
-      <c r="M11" s="122">
+      <c r="M11" s="114">
         <v>0.26666666666666666</v>
       </c>
-      <c r="N11" s="123" t="s">
+      <c r="N11" s="116" t="s">
         <v>58</v>
       </c>
-      <c r="O11" s="114" t="s">
+      <c r="O11" s="118" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="12" spans="2:15" ht="21.75" customHeight="1" thickBot="1">
-      <c r="B12" s="117"/>
-      <c r="C12" s="101"/>
-      <c r="D12" s="101"/>
-      <c r="E12" s="101"/>
-      <c r="F12" s="101"/>
-      <c r="G12" s="126"/>
-      <c r="H12" s="101"/>
-      <c r="I12" s="101"/>
-      <c r="J12" s="101"/>
-      <c r="K12" s="101"/>
-      <c r="L12" s="120"/>
-      <c r="M12" s="121"/>
-      <c r="N12" s="124"/>
-      <c r="O12" s="115"/>
+      <c r="B12" s="124"/>
+      <c r="C12" s="105"/>
+      <c r="D12" s="105"/>
+      <c r="E12" s="105"/>
+      <c r="F12" s="105"/>
+      <c r="G12" s="121"/>
+      <c r="H12" s="105"/>
+      <c r="I12" s="105"/>
+      <c r="J12" s="105"/>
+      <c r="K12" s="105"/>
+      <c r="L12" s="126"/>
+      <c r="M12" s="115"/>
+      <c r="N12" s="117"/>
+      <c r="O12" s="119"/>
     </row>
     <row r="13" spans="2:15" ht="22.5" customHeight="1">
-      <c r="B13" s="116" t="s">
+      <c r="B13" s="123" t="s">
         <v>96</v>
       </c>
-      <c r="C13" s="100" t="s">
+      <c r="C13" s="96" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="100" t="s">
+      <c r="D13" s="96" t="s">
         <v>41</v>
       </c>
-      <c r="E13" s="100" t="s">
+      <c r="E13" s="96" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="118" t="s">
+      <c r="F13" s="122" t="s">
         <v>36</v>
       </c>
-      <c r="G13" s="100" t="s">
+      <c r="G13" s="96" t="s">
         <v>41</v>
       </c>
-      <c r="H13" s="125"/>
-      <c r="I13" s="118" t="s">
+      <c r="H13" s="120"/>
+      <c r="I13" s="122" t="s">
         <v>36</v>
       </c>
-      <c r="J13" s="118" t="s">
+      <c r="J13" s="122" t="s">
         <v>36</v>
       </c>
-      <c r="K13" s="118" t="s">
+      <c r="K13" s="122" t="s">
         <v>55</v>
       </c>
-      <c r="L13" s="119" t="s">
+      <c r="L13" s="125" t="s">
         <v>55</v>
       </c>
-      <c r="M13" s="121"/>
-      <c r="N13" s="123" t="s">
+      <c r="M13" s="115"/>
+      <c r="N13" s="116" t="s">
         <v>42</v>
       </c>
-      <c r="O13" s="114" t="s">
+      <c r="O13" s="118" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="14" spans="2:15" ht="22.5" customHeight="1" thickBot="1">
-      <c r="B14" s="117"/>
-      <c r="C14" s="101"/>
-      <c r="D14" s="101"/>
-      <c r="E14" s="101"/>
-      <c r="F14" s="101"/>
-      <c r="G14" s="101"/>
-      <c r="H14" s="126"/>
-      <c r="I14" s="101"/>
-      <c r="J14" s="101"/>
-      <c r="K14" s="101"/>
-      <c r="L14" s="120"/>
-      <c r="M14" s="121"/>
-      <c r="N14" s="124"/>
-      <c r="O14" s="115"/>
+      <c r="B14" s="124"/>
+      <c r="C14" s="105"/>
+      <c r="D14" s="105"/>
+      <c r="E14" s="105"/>
+      <c r="F14" s="105"/>
+      <c r="G14" s="105"/>
+      <c r="H14" s="121"/>
+      <c r="I14" s="105"/>
+      <c r="J14" s="105"/>
+      <c r="K14" s="105"/>
+      <c r="L14" s="126"/>
+      <c r="M14" s="115"/>
+      <c r="N14" s="117"/>
+      <c r="O14" s="119"/>
     </row>
     <row r="15" spans="2:15" ht="22.5" customHeight="1">
-      <c r="B15" s="116" t="s">
+      <c r="B15" s="123" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="118" t="s">
+      <c r="C15" s="122" t="s">
         <v>41</v>
       </c>
-      <c r="D15" s="100" t="s">
+      <c r="D15" s="96" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="100" t="s">
+      <c r="E15" s="96" t="s">
         <v>41</v>
       </c>
-      <c r="F15" s="100" t="s">
+      <c r="F15" s="96" t="s">
         <v>41</v>
       </c>
-      <c r="G15" s="118" t="s">
+      <c r="G15" s="122" t="s">
         <v>36</v>
       </c>
-      <c r="H15" s="100" t="s">
+      <c r="H15" s="96" t="s">
         <v>41</v>
       </c>
-      <c r="I15" s="125"/>
-      <c r="J15" s="118" t="s">
+      <c r="I15" s="120"/>
+      <c r="J15" s="122" t="s">
         <v>36</v>
       </c>
-      <c r="K15" s="100" t="s">
+      <c r="K15" s="96" t="s">
         <v>41</v>
       </c>
-      <c r="L15" s="119" t="s">
+      <c r="L15" s="125" t="s">
         <v>55</v>
       </c>
-      <c r="M15" s="122">
+      <c r="M15" s="114">
         <v>0.34583333333333338</v>
       </c>
-      <c r="N15" s="123" t="s">
+      <c r="N15" s="116" t="s">
         <v>57</v>
       </c>
-      <c r="O15" s="114" t="s">
+      <c r="O15" s="118" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="16" spans="2:15" ht="22.5" customHeight="1" thickBot="1">
-      <c r="B16" s="117"/>
-      <c r="C16" s="101"/>
-      <c r="D16" s="101"/>
-      <c r="E16" s="101"/>
-      <c r="F16" s="101"/>
-      <c r="G16" s="101"/>
-      <c r="H16" s="101"/>
-      <c r="I16" s="126"/>
-      <c r="J16" s="101"/>
-      <c r="K16" s="101"/>
-      <c r="L16" s="120"/>
-      <c r="M16" s="121"/>
-      <c r="N16" s="124"/>
-      <c r="O16" s="115"/>
+      <c r="B16" s="124"/>
+      <c r="C16" s="105"/>
+      <c r="D16" s="105"/>
+      <c r="E16" s="105"/>
+      <c r="F16" s="105"/>
+      <c r="G16" s="105"/>
+      <c r="H16" s="105"/>
+      <c r="I16" s="121"/>
+      <c r="J16" s="105"/>
+      <c r="K16" s="105"/>
+      <c r="L16" s="126"/>
+      <c r="M16" s="115"/>
+      <c r="N16" s="117"/>
+      <c r="O16" s="119"/>
     </row>
     <row r="17" spans="2:15" ht="21.75" customHeight="1">
-      <c r="B17" s="116" t="s">
+      <c r="B17" s="123" t="s">
         <v>97</v>
       </c>
-      <c r="C17" s="100" t="s">
+      <c r="C17" s="96" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="100" t="s">
+      <c r="D17" s="96" t="s">
         <v>41</v>
       </c>
-      <c r="E17" s="100" t="s">
+      <c r="E17" s="96" t="s">
         <v>41</v>
       </c>
-      <c r="F17" s="100" t="s">
+      <c r="F17" s="96" t="s">
         <v>41</v>
       </c>
-      <c r="G17" s="100" t="s">
+      <c r="G17" s="96" t="s">
         <v>41</v>
       </c>
-      <c r="H17" s="118" t="s">
+      <c r="H17" s="122" t="s">
         <v>41</v>
       </c>
-      <c r="I17" s="100" t="s">
+      <c r="I17" s="96" t="s">
         <v>41</v>
       </c>
-      <c r="J17" s="125"/>
-      <c r="K17" s="118" t="s">
+      <c r="J17" s="120"/>
+      <c r="K17" s="122" t="s">
         <v>41</v>
       </c>
-      <c r="L17" s="119" t="s">
+      <c r="L17" s="125" t="s">
         <v>55</v>
       </c>
-      <c r="M17" s="121"/>
-      <c r="N17" s="123" t="s">
+      <c r="M17" s="115"/>
+      <c r="N17" s="116" t="s">
         <v>43</v>
       </c>
-      <c r="O17" s="114" t="s">
+      <c r="O17" s="118" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="18" spans="2:15" ht="21.75" customHeight="1" thickBot="1">
-      <c r="B18" s="117"/>
-      <c r="C18" s="101"/>
-      <c r="D18" s="101"/>
-      <c r="E18" s="101"/>
-      <c r="F18" s="101"/>
-      <c r="G18" s="101"/>
-      <c r="H18" s="101"/>
-      <c r="I18" s="101"/>
-      <c r="J18" s="126"/>
-      <c r="K18" s="101"/>
-      <c r="L18" s="120"/>
-      <c r="M18" s="121"/>
-      <c r="N18" s="124"/>
-      <c r="O18" s="115"/>
+      <c r="B18" s="124"/>
+      <c r="C18" s="105"/>
+      <c r="D18" s="105"/>
+      <c r="E18" s="105"/>
+      <c r="F18" s="105"/>
+      <c r="G18" s="105"/>
+      <c r="H18" s="105"/>
+      <c r="I18" s="105"/>
+      <c r="J18" s="121"/>
+      <c r="K18" s="105"/>
+      <c r="L18" s="126"/>
+      <c r="M18" s="115"/>
+      <c r="N18" s="117"/>
+      <c r="O18" s="119"/>
     </row>
     <row r="19" spans="2:15" ht="21.75" customHeight="1">
-      <c r="B19" s="116" t="s">
+      <c r="B19" s="123" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="118" t="s">
+      <c r="C19" s="122" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="118" t="s">
+      <c r="D19" s="122" t="s">
         <v>36</v>
       </c>
-      <c r="E19" s="118" t="s">
+      <c r="E19" s="122" t="s">
         <v>39</v>
       </c>
-      <c r="F19" s="118" t="s">
+      <c r="F19" s="122" t="s">
         <v>41</v>
       </c>
-      <c r="G19" s="118" t="s">
+      <c r="G19" s="122" t="s">
         <v>36</v>
       </c>
-      <c r="H19" s="118" t="s">
+      <c r="H19" s="122" t="s">
         <v>52</v>
       </c>
-      <c r="I19" s="118" t="s">
+      <c r="I19" s="122" t="s">
         <v>36</v>
       </c>
-      <c r="J19" s="118" t="s">
+      <c r="J19" s="122" t="s">
         <v>36</v>
       </c>
-      <c r="K19" s="125"/>
-      <c r="L19" s="119" t="s">
+      <c r="K19" s="120"/>
+      <c r="L19" s="125" t="s">
         <v>36</v>
       </c>
-      <c r="M19" s="121"/>
-      <c r="N19" s="123" t="s">
+      <c r="M19" s="115"/>
+      <c r="N19" s="116" t="s">
         <v>45</v>
       </c>
-      <c r="O19" s="114" t="s">
+      <c r="O19" s="118" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="20" spans="2:15" ht="22.5" customHeight="1" thickBot="1">
-      <c r="B20" s="117"/>
-      <c r="C20" s="101"/>
-      <c r="D20" s="101"/>
-      <c r="E20" s="101"/>
-      <c r="F20" s="101"/>
-      <c r="G20" s="101"/>
-      <c r="H20" s="101"/>
-      <c r="I20" s="101"/>
-      <c r="J20" s="101"/>
-      <c r="K20" s="126"/>
-      <c r="L20" s="120"/>
-      <c r="M20" s="121"/>
-      <c r="N20" s="124"/>
-      <c r="O20" s="115"/>
+      <c r="B20" s="124"/>
+      <c r="C20" s="105"/>
+      <c r="D20" s="105"/>
+      <c r="E20" s="105"/>
+      <c r="F20" s="105"/>
+      <c r="G20" s="105"/>
+      <c r="H20" s="105"/>
+      <c r="I20" s="105"/>
+      <c r="J20" s="105"/>
+      <c r="K20" s="121"/>
+      <c r="L20" s="126"/>
+      <c r="M20" s="115"/>
+      <c r="N20" s="117"/>
+      <c r="O20" s="119"/>
     </row>
     <row r="21" spans="2:15" ht="22.5" customHeight="1">
-      <c r="B21" s="134" t="s">
+      <c r="B21" s="130" t="s">
         <v>98</v>
       </c>
-      <c r="C21" s="100" t="s">
+      <c r="C21" s="96" t="s">
         <v>41</v>
       </c>
-      <c r="D21" s="100" t="s">
+      <c r="D21" s="96" t="s">
         <v>41</v>
       </c>
-      <c r="E21" s="100" t="s">
+      <c r="E21" s="96" t="s">
         <v>41</v>
       </c>
-      <c r="F21" s="100" t="s">
+      <c r="F21" s="96" t="s">
         <v>41</v>
       </c>
-      <c r="G21" s="118" t="s">
+      <c r="G21" s="122" t="s">
         <v>52</v>
       </c>
-      <c r="H21" s="118" t="s">
+      <c r="H21" s="122" t="s">
         <v>52</v>
       </c>
-      <c r="I21" s="118" t="s">
+      <c r="I21" s="122" t="s">
         <v>52</v>
       </c>
-      <c r="J21" s="118" t="s">
+      <c r="J21" s="122" t="s">
         <v>52</v>
       </c>
-      <c r="K21" s="100" t="s">
+      <c r="K21" s="96" t="s">
         <v>41</v>
       </c>
-      <c r="L21" s="125"/>
-      <c r="M21" s="122">
+      <c r="L21" s="120"/>
+      <c r="M21" s="114">
         <v>0.51597222222222217</v>
       </c>
-      <c r="N21" s="123" t="s">
+      <c r="N21" s="116" t="s">
         <v>60</v>
       </c>
-      <c r="O21" s="114" t="s">
+      <c r="O21" s="118" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="22" spans="2:15" ht="15" thickBot="1">
-      <c r="B22" s="135"/>
-      <c r="C22" s="131"/>
-      <c r="D22" s="131"/>
-      <c r="E22" s="131"/>
-      <c r="F22" s="131"/>
-      <c r="G22" s="131"/>
-      <c r="H22" s="131"/>
-      <c r="I22" s="131"/>
-      <c r="J22" s="131"/>
-      <c r="K22" s="131"/>
-      <c r="L22" s="132"/>
-      <c r="M22" s="133"/>
-      <c r="N22" s="129"/>
-      <c r="O22" s="130"/>
+      <c r="B22" s="131"/>
+      <c r="C22" s="129"/>
+      <c r="D22" s="129"/>
+      <c r="E22" s="129"/>
+      <c r="F22" s="129"/>
+      <c r="G22" s="129"/>
+      <c r="H22" s="129"/>
+      <c r="I22" s="129"/>
+      <c r="J22" s="129"/>
+      <c r="K22" s="129"/>
+      <c r="L22" s="134"/>
+      <c r="M22" s="135"/>
+      <c r="N22" s="132"/>
+      <c r="O22" s="133"/>
     </row>
   </sheetData>
   <mergeCells count="140">
@@ -4213,6 +4250,9 @@
     <mergeCell ref="H15:H16"/>
     <mergeCell ref="L13:L14"/>
     <mergeCell ref="M13:M14"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="K9:K10"/>
     <mergeCell ref="N13:N14"/>
     <mergeCell ref="O13:O14"/>
     <mergeCell ref="C11:C12"/>
@@ -4222,38 +4262,36 @@
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="H11:H12"/>
     <mergeCell ref="O11:O12"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:H8"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="D9:D10"/>
     <mergeCell ref="E9:E10"/>
     <mergeCell ref="F9:F10"/>
     <mergeCell ref="G9:G10"/>
     <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="M11:M12"/>
-    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="O3:O4"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="N3:N4"/>
+    <mergeCell ref="L5:L6"/>
     <mergeCell ref="L9:L10"/>
     <mergeCell ref="M9:M10"/>
     <mergeCell ref="N9:N10"/>
     <mergeCell ref="O9:O10"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="O7:O8"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
     <mergeCell ref="H5:H6"/>
     <mergeCell ref="I5:I6"/>
     <mergeCell ref="J5:J6"/>
@@ -4263,8 +4301,14 @@
     <mergeCell ref="K7:K8"/>
     <mergeCell ref="L7:L8"/>
     <mergeCell ref="M7:M8"/>
-    <mergeCell ref="N7:N8"/>
-    <mergeCell ref="O3:O4"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="O5:O6"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="B13:B14"/>
@@ -4274,20 +4318,13 @@
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="I3:I4"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="M3:M4"/>
-    <mergeCell ref="N3:N4"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="O5:O6"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="O7:O8"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4354,29 +4391,29 @@
       <c r="A5" s="142">
         <v>1</v>
       </c>
-      <c r="B5" s="106" t="s">
+      <c r="B5" s="107" t="s">
         <v>102</v>
       </c>
       <c r="C5" s="63"/>
-      <c r="D5" s="170" t="s">
+      <c r="D5" s="167" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="158" t="s">
+      <c r="E5" s="172" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="176" t="s">
+      <c r="F5" s="175" t="s">
         <v>35</v>
       </c>
-      <c r="G5" s="158" t="s">
+      <c r="G5" s="172" t="s">
         <v>52</v>
       </c>
-      <c r="H5" s="100" t="s">
+      <c r="H5" s="96" t="s">
         <v>36</v>
       </c>
       <c r="I5" s="138" t="s">
         <v>36</v>
       </c>
-      <c r="J5" s="119" t="s">
+      <c r="J5" s="125" t="s">
         <v>110</v>
       </c>
       <c r="K5" s="141" t="s">
@@ -4396,14 +4433,14 @@
         <v>103</v>
       </c>
       <c r="C6" s="147"/>
-      <c r="D6" s="164"/>
-      <c r="E6" s="88"/>
-      <c r="F6" s="149"/>
-      <c r="G6" s="88"/>
-      <c r="H6" s="90"/>
-      <c r="I6" s="90"/>
-      <c r="J6" s="70"/>
-      <c r="K6" s="88"/>
+      <c r="D6" s="168"/>
+      <c r="E6" s="94"/>
+      <c r="F6" s="174"/>
+      <c r="G6" s="94"/>
+      <c r="H6" s="99"/>
+      <c r="I6" s="99"/>
+      <c r="J6" s="67"/>
+      <c r="K6" s="94"/>
       <c r="L6" s="140"/>
       <c r="M6" s="28"/>
       <c r="N6" s="28"/>
@@ -4414,29 +4451,29 @@
       <c r="A7" s="142">
         <v>2</v>
       </c>
-      <c r="B7" s="106" t="s">
+      <c r="B7" s="107" t="s">
         <v>104</v>
       </c>
       <c r="C7" s="63"/>
-      <c r="D7" s="171" t="s">
+      <c r="D7" s="169" t="s">
         <v>41</v>
       </c>
-      <c r="E7" s="85" t="s">
+      <c r="E7" s="100" t="s">
         <v>51</v>
       </c>
-      <c r="F7" s="175" t="s">
+      <c r="F7" s="173" t="s">
         <v>41</v>
       </c>
-      <c r="G7" s="150" t="s">
+      <c r="G7" s="176" t="s">
         <v>41</v>
       </c>
-      <c r="H7" s="118" t="s">
+      <c r="H7" s="122" t="s">
         <v>41</v>
       </c>
-      <c r="I7" s="118" t="s">
+      <c r="I7" s="122" t="s">
         <v>55</v>
       </c>
-      <c r="J7" s="119" t="s">
+      <c r="J7" s="125" t="s">
         <v>111</v>
       </c>
       <c r="K7" s="145" t="s">
@@ -4456,14 +4493,14 @@
         <v>53</v>
       </c>
       <c r="C8" s="147"/>
-      <c r="D8" s="172"/>
-      <c r="E8" s="86"/>
-      <c r="F8" s="149"/>
-      <c r="G8" s="88"/>
-      <c r="H8" s="103"/>
-      <c r="I8" s="103"/>
+      <c r="D8" s="170"/>
+      <c r="E8" s="95"/>
+      <c r="F8" s="174"/>
+      <c r="G8" s="94"/>
+      <c r="H8" s="97"/>
+      <c r="I8" s="97"/>
       <c r="J8" s="63"/>
-      <c r="K8" s="88"/>
+      <c r="K8" s="94"/>
       <c r="L8" s="144"/>
       <c r="M8" s="28"/>
       <c r="N8" s="28"/>
@@ -4474,35 +4511,35 @@
       <c r="A9" s="142">
         <v>3</v>
       </c>
-      <c r="B9" s="106" t="s">
+      <c r="B9" s="107" t="s">
         <v>105</v>
       </c>
       <c r="C9" s="63"/>
       <c r="D9" s="178" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="151" t="s">
+      <c r="E9" s="161" t="s">
         <v>36</v>
       </c>
-      <c r="F9" s="148" t="s">
+      <c r="F9" s="177" t="s">
         <v>51</v>
       </c>
-      <c r="G9" s="150" t="s">
+      <c r="G9" s="176" t="s">
         <v>39</v>
       </c>
-      <c r="H9" s="151" t="s">
+      <c r="H9" s="161" t="s">
         <v>35</v>
       </c>
-      <c r="I9" s="151" t="s">
+      <c r="I9" s="161" t="s">
         <v>36</v>
       </c>
-      <c r="J9" s="174" t="s">
+      <c r="J9" s="159" t="s">
         <v>56</v>
       </c>
       <c r="K9" s="145" t="s">
         <v>42</v>
       </c>
-      <c r="L9" s="177" t="s">
+      <c r="L9" s="160" t="s">
         <v>42</v>
       </c>
       <c r="M9" s="28"/>
@@ -4511,19 +4548,19 @@
       <c r="P9" s="28"/>
     </row>
     <row r="10" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A10" s="164"/>
-      <c r="B10" s="159" t="s">
+      <c r="A10" s="168"/>
+      <c r="B10" s="154" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="63"/>
-      <c r="D10" s="164"/>
-      <c r="E10" s="90"/>
-      <c r="F10" s="149"/>
-      <c r="G10" s="88"/>
-      <c r="H10" s="90"/>
-      <c r="I10" s="90"/>
-      <c r="J10" s="70"/>
-      <c r="K10" s="88"/>
+      <c r="D10" s="168"/>
+      <c r="E10" s="99"/>
+      <c r="F10" s="174"/>
+      <c r="G10" s="94"/>
+      <c r="H10" s="99"/>
+      <c r="I10" s="99"/>
+      <c r="J10" s="67"/>
+      <c r="K10" s="94"/>
       <c r="L10" s="140"/>
       <c r="M10" s="28"/>
       <c r="N10" s="28"/>
@@ -4531,32 +4568,32 @@
       <c r="P10" s="28"/>
     </row>
     <row r="11" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A11" s="165">
+      <c r="A11" s="162">
         <v>4</v>
       </c>
-      <c r="B11" s="160" t="s">
+      <c r="B11" s="155" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="161"/>
-      <c r="D11" s="173" t="s">
+      <c r="C11" s="156"/>
+      <c r="D11" s="171" t="s">
         <v>55</v>
       </c>
       <c r="E11" s="141" t="s">
         <v>36</v>
       </c>
-      <c r="F11" s="119" t="s">
+      <c r="F11" s="125" t="s">
         <v>35</v>
       </c>
-      <c r="G11" s="105" t="s">
+      <c r="G11" s="106" t="s">
         <v>51</v>
       </c>
-      <c r="H11" s="118" t="s">
+      <c r="H11" s="122" t="s">
         <v>52</v>
       </c>
-      <c r="I11" s="118" t="s">
+      <c r="I11" s="122" t="s">
         <v>36</v>
       </c>
-      <c r="J11" s="119" t="s">
+      <c r="J11" s="125" t="s">
         <v>109</v>
       </c>
       <c r="K11" s="145" t="s">
@@ -4571,52 +4608,52 @@
       <c r="P11" s="28"/>
     </row>
     <row r="12" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A12" s="166"/>
-      <c r="B12" s="162" t="s">
+      <c r="A12" s="163"/>
+      <c r="B12" s="157" t="s">
         <v>15</v>
       </c>
       <c r="C12" s="63"/>
-      <c r="D12" s="164"/>
-      <c r="E12" s="88"/>
-      <c r="F12" s="70"/>
-      <c r="G12" s="88"/>
-      <c r="H12" s="90"/>
-      <c r="I12" s="90"/>
-      <c r="J12" s="70"/>
-      <c r="K12" s="88"/>
-      <c r="L12" s="88"/>
+      <c r="D12" s="168"/>
+      <c r="E12" s="94"/>
+      <c r="F12" s="67"/>
+      <c r="G12" s="94"/>
+      <c r="H12" s="99"/>
+      <c r="I12" s="99"/>
+      <c r="J12" s="67"/>
+      <c r="K12" s="94"/>
+      <c r="L12" s="94"/>
       <c r="M12" s="28"/>
       <c r="N12" s="28"/>
       <c r="O12" s="28"/>
       <c r="P12" s="28"/>
     </row>
     <row r="13" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A13" s="165" t="s">
+      <c r="A13" s="162" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="160" t="s">
+      <c r="B13" s="155" t="s">
         <v>98</v>
       </c>
-      <c r="C13" s="163"/>
-      <c r="D13" s="89" t="s">
+      <c r="C13" s="158"/>
+      <c r="D13" s="98" t="s">
         <v>41</v>
       </c>
       <c r="E13" s="145" t="s">
         <v>36</v>
       </c>
-      <c r="F13" s="174" t="s">
+      <c r="F13" s="159" t="s">
         <v>39</v>
       </c>
       <c r="G13" s="145" t="s">
         <v>55</v>
       </c>
-      <c r="H13" s="105" t="s">
+      <c r="H13" s="106" t="s">
         <v>51</v>
       </c>
-      <c r="I13" s="151" t="s">
+      <c r="I13" s="161" t="s">
         <v>52</v>
       </c>
-      <c r="J13" s="174" t="s">
+      <c r="J13" s="159" t="s">
         <v>108</v>
       </c>
       <c r="K13" s="145" t="s">
@@ -4632,19 +4669,19 @@
     </row>
     <row r="14" spans="1:16" ht="15.75" customHeight="1">
       <c r="A14" s="143"/>
-      <c r="B14" s="167" t="s">
+      <c r="B14" s="164" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="168"/>
-      <c r="D14" s="90"/>
-      <c r="E14" s="88"/>
-      <c r="F14" s="70"/>
-      <c r="G14" s="88"/>
-      <c r="H14" s="88"/>
-      <c r="I14" s="90"/>
-      <c r="J14" s="70"/>
-      <c r="K14" s="88"/>
-      <c r="L14" s="88"/>
+      <c r="C14" s="165"/>
+      <c r="D14" s="99"/>
+      <c r="E14" s="94"/>
+      <c r="F14" s="67"/>
+      <c r="G14" s="94"/>
+      <c r="H14" s="94"/>
+      <c r="I14" s="99"/>
+      <c r="J14" s="67"/>
+      <c r="K14" s="94"/>
+      <c r="L14" s="94"/>
       <c r="M14" s="28"/>
       <c r="N14" s="28"/>
       <c r="O14" s="28"/>
@@ -4654,29 +4691,29 @@
       <c r="A15" s="142" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="106" t="s">
+      <c r="B15" s="107" t="s">
         <v>106</v>
       </c>
       <c r="C15" s="63"/>
-      <c r="D15" s="170" t="s">
+      <c r="D15" s="167" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="158" t="s">
+      <c r="E15" s="172" t="s">
         <v>52</v>
       </c>
-      <c r="F15" s="176" t="s">
+      <c r="F15" s="175" t="s">
         <v>41</v>
       </c>
-      <c r="G15" s="158" t="s">
+      <c r="G15" s="172" t="s">
         <v>41</v>
       </c>
-      <c r="H15" s="118" t="s">
+      <c r="H15" s="122" t="s">
         <v>55</v>
       </c>
       <c r="I15" s="138" t="s">
         <v>51</v>
       </c>
-      <c r="J15" s="119" t="s">
+      <c r="J15" s="125" t="s">
         <v>107</v>
       </c>
       <c r="K15" s="141" t="s">
@@ -4692,45 +4729,45 @@
     </row>
     <row r="16" spans="1:16" ht="15.75" customHeight="1">
       <c r="A16" s="143"/>
-      <c r="B16" s="169" t="s">
+      <c r="B16" s="166" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="70"/>
-      <c r="D16" s="164"/>
-      <c r="E16" s="88"/>
-      <c r="F16" s="149"/>
-      <c r="G16" s="88"/>
-      <c r="H16" s="90"/>
-      <c r="I16" s="90"/>
-      <c r="J16" s="70"/>
-      <c r="K16" s="88"/>
-      <c r="L16" s="88"/>
+      <c r="C16" s="67"/>
+      <c r="D16" s="168"/>
+      <c r="E16" s="94"/>
+      <c r="F16" s="174"/>
+      <c r="G16" s="94"/>
+      <c r="H16" s="99"/>
+      <c r="I16" s="99"/>
+      <c r="J16" s="67"/>
+      <c r="K16" s="94"/>
+      <c r="L16" s="94"/>
       <c r="M16" s="28"/>
       <c r="N16" s="28"/>
       <c r="O16" s="28"/>
       <c r="P16" s="28"/>
     </row>
     <row r="17" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A17" s="154"/>
-      <c r="B17" s="152"/>
+      <c r="A17" s="148"/>
+      <c r="B17" s="153"/>
       <c r="C17" s="63"/>
-      <c r="D17" s="155"/>
-      <c r="E17" s="157"/>
-      <c r="F17" s="156"/>
-      <c r="G17" s="156"/>
-      <c r="H17" s="155"/>
-      <c r="I17" s="155"/>
-      <c r="J17" s="157"/>
-      <c r="K17" s="156"/>
-      <c r="L17" s="156"/>
-      <c r="M17" s="155"/>
-      <c r="N17" s="155"/>
-      <c r="O17" s="155"/>
-      <c r="P17" s="155"/>
+      <c r="D17" s="149"/>
+      <c r="E17" s="151"/>
+      <c r="F17" s="150"/>
+      <c r="G17" s="150"/>
+      <c r="H17" s="149"/>
+      <c r="I17" s="149"/>
+      <c r="J17" s="151"/>
+      <c r="K17" s="150"/>
+      <c r="L17" s="150"/>
+      <c r="M17" s="149"/>
+      <c r="N17" s="149"/>
+      <c r="O17" s="149"/>
+      <c r="P17" s="149"/>
     </row>
     <row r="18" spans="1:16" ht="15.75" customHeight="1">
       <c r="A18" s="63"/>
-      <c r="B18" s="153"/>
+      <c r="B18" s="152"/>
       <c r="C18" s="63"/>
       <c r="D18" s="63"/>
       <c r="E18" s="63"/>
@@ -4747,26 +4784,26 @@
       <c r="P18" s="63"/>
     </row>
     <row r="19" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A19" s="154"/>
-      <c r="B19" s="152"/>
+      <c r="A19" s="148"/>
+      <c r="B19" s="153"/>
       <c r="C19" s="63"/>
-      <c r="D19" s="155"/>
-      <c r="E19" s="155"/>
-      <c r="F19" s="157"/>
-      <c r="G19" s="156"/>
-      <c r="H19" s="155"/>
-      <c r="I19" s="155"/>
-      <c r="J19" s="155"/>
-      <c r="K19" s="157"/>
-      <c r="L19" s="156"/>
-      <c r="M19" s="155"/>
-      <c r="N19" s="155"/>
-      <c r="O19" s="155"/>
-      <c r="P19" s="155"/>
+      <c r="D19" s="149"/>
+      <c r="E19" s="149"/>
+      <c r="F19" s="151"/>
+      <c r="G19" s="150"/>
+      <c r="H19" s="149"/>
+      <c r="I19" s="149"/>
+      <c r="J19" s="149"/>
+      <c r="K19" s="151"/>
+      <c r="L19" s="150"/>
+      <c r="M19" s="149"/>
+      <c r="N19" s="149"/>
+      <c r="O19" s="149"/>
+      <c r="P19" s="149"/>
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1">
       <c r="A20" s="63"/>
-      <c r="B20" s="153"/>
+      <c r="B20" s="152"/>
       <c r="C20" s="63"/>
       <c r="D20" s="63"/>
       <c r="E20" s="63"/>
@@ -4783,26 +4820,26 @@
       <c r="P20" s="63"/>
     </row>
     <row r="21" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A21" s="154"/>
-      <c r="B21" s="152"/>
+      <c r="A21" s="148"/>
+      <c r="B21" s="153"/>
       <c r="C21" s="63"/>
-      <c r="D21" s="155"/>
-      <c r="E21" s="155"/>
-      <c r="F21" s="155"/>
-      <c r="G21" s="157"/>
-      <c r="H21" s="155"/>
-      <c r="I21" s="155"/>
-      <c r="J21" s="155"/>
-      <c r="K21" s="155"/>
-      <c r="L21" s="157"/>
-      <c r="M21" s="155"/>
-      <c r="N21" s="155"/>
-      <c r="O21" s="155"/>
-      <c r="P21" s="155"/>
+      <c r="D21" s="149"/>
+      <c r="E21" s="149"/>
+      <c r="F21" s="149"/>
+      <c r="G21" s="151"/>
+      <c r="H21" s="149"/>
+      <c r="I21" s="149"/>
+      <c r="J21" s="149"/>
+      <c r="K21" s="149"/>
+      <c r="L21" s="151"/>
+      <c r="M21" s="149"/>
+      <c r="N21" s="149"/>
+      <c r="O21" s="149"/>
+      <c r="P21" s="149"/>
     </row>
     <row r="22" spans="1:16" ht="15.75" customHeight="1">
       <c r="A22" s="63"/>
-      <c r="B22" s="153"/>
+      <c r="B22" s="152"/>
       <c r="C22" s="63"/>
       <c r="D22" s="63"/>
       <c r="E22" s="63"/>
@@ -4819,26 +4856,26 @@
       <c r="P22" s="63"/>
     </row>
     <row r="23" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A23" s="154"/>
-      <c r="B23" s="152"/>
+      <c r="A23" s="148"/>
+      <c r="B23" s="153"/>
       <c r="C23" s="63"/>
-      <c r="D23" s="155"/>
-      <c r="E23" s="155"/>
-      <c r="F23" s="155"/>
-      <c r="G23" s="155"/>
-      <c r="H23" s="157"/>
-      <c r="I23" s="155"/>
-      <c r="J23" s="155"/>
-      <c r="K23" s="155"/>
-      <c r="L23" s="155"/>
-      <c r="M23" s="157"/>
-      <c r="N23" s="155"/>
-      <c r="O23" s="155"/>
-      <c r="P23" s="155"/>
+      <c r="D23" s="149"/>
+      <c r="E23" s="149"/>
+      <c r="F23" s="149"/>
+      <c r="G23" s="149"/>
+      <c r="H23" s="151"/>
+      <c r="I23" s="149"/>
+      <c r="J23" s="149"/>
+      <c r="K23" s="149"/>
+      <c r="L23" s="149"/>
+      <c r="M23" s="151"/>
+      <c r="N23" s="149"/>
+      <c r="O23" s="149"/>
+      <c r="P23" s="149"/>
     </row>
     <row r="24" spans="1:16" ht="15.75" customHeight="1">
       <c r="A24" s="63"/>
-      <c r="B24" s="153"/>
+      <c r="B24" s="152"/>
       <c r="C24" s="63"/>
       <c r="D24" s="63"/>
       <c r="E24" s="63"/>
@@ -4857,10 +4894,6 @@
     <row r="25" spans="1:16" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="137">
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="H11:H12"/>
     <mergeCell ref="K13:K14"/>
     <mergeCell ref="J13:J14"/>
     <mergeCell ref="L13:L14"/>
@@ -4870,15 +4903,18 @@
     <mergeCell ref="I13:I14"/>
     <mergeCell ref="J15:J16"/>
     <mergeCell ref="K11:K12"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="E13:E14"/>
     <mergeCell ref="F15:F16"/>
     <mergeCell ref="E15:E16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="H9:H10"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="B14:C14"/>
@@ -4889,8 +4925,9 @@
     <mergeCell ref="D13:D14"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="D15:D16"/>
-    <mergeCell ref="P21:P22"/>
-    <mergeCell ref="O21:O22"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:C9"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="I21:I22"/>
     <mergeCell ref="J21:J22"/>
@@ -4913,10 +4950,8 @@
     <mergeCell ref="L11:L12"/>
     <mergeCell ref="L9:L10"/>
     <mergeCell ref="I9:I10"/>
-    <mergeCell ref="O19:O20"/>
-    <mergeCell ref="P19:P20"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="E13:E14"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="E19:E20"/>
     <mergeCell ref="E17:E18"/>
@@ -4926,14 +4961,10 @@
     <mergeCell ref="M17:M18"/>
     <mergeCell ref="O17:O18"/>
     <mergeCell ref="P17:P18"/>
-    <mergeCell ref="H15:H16"/>
     <mergeCell ref="H17:H18"/>
     <mergeCell ref="G17:G18"/>
-    <mergeCell ref="G15:G16"/>
     <mergeCell ref="H19:H20"/>
     <mergeCell ref="J19:J20"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="F21:F22"/>
     <mergeCell ref="N21:N22"/>
     <mergeCell ref="M21:M22"/>
     <mergeCell ref="N19:N20"/>
@@ -4941,6 +4972,10 @@
     <mergeCell ref="I19:I20"/>
     <mergeCell ref="N23:N24"/>
     <mergeCell ref="O23:O24"/>
+    <mergeCell ref="O19:O20"/>
+    <mergeCell ref="P19:P20"/>
+    <mergeCell ref="P21:P22"/>
+    <mergeCell ref="O21:O22"/>
     <mergeCell ref="P23:P24"/>
     <mergeCell ref="M23:M24"/>
     <mergeCell ref="H23:H24"/>
@@ -4970,8 +5005,10 @@
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="E21:E22"/>
     <mergeCell ref="D21:D22"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="D19:D20"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="I5:I6"/>
@@ -4988,12 +5025,12 @@
     <mergeCell ref="J7:J8"/>
     <mergeCell ref="H7:H8"/>
     <mergeCell ref="I7:I8"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:G10"/>
     <mergeCell ref="H5:H6"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="G7:G8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5001,31 +5038,55 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D0CA921-B84F-45E1-B6F9-B23EA2C5E3C9}">
-  <dimension ref="B1:C3"/>
+  <dimension ref="B1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="2" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3">
+    <row r="1" spans="2:4">
       <c r="B1" s="60" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="2:3">
+    <row r="2" spans="2:4">
       <c r="B2" s="59"/>
       <c r="C2" s="60" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="2:3">
+    <row r="3" spans="2:4">
       <c r="B3" s="61" t="s">
         <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="15" thickBot="1"/>
+    <row r="5" spans="2:4">
+      <c r="B5" s="183" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="181" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" s="179" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" ht="15" thickBot="1">
+      <c r="B6" s="184" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="182" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="180" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>